<commit_message>
Added vwap, adtv and rolling vola calcs
</commit_message>
<xml_diff>
--- a/vwap.xlsx
+++ b/vwap.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\top kek\Desktop\Python\2_External APIs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B15A71-3D1A-4ACC-A030-083DD9F11BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="24468" yWindow="-1308" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>p</t>
   </si>
@@ -23,6 +40,15 @@
   </si>
   <si>
     <t>vwap</t>
+  </si>
+  <si>
+    <t>adtv30d</t>
+  </si>
+  <si>
+    <t>adtv90d</t>
+  </si>
+  <si>
+    <t>vola</t>
   </si>
   <si>
     <t>date</t>
@@ -319,8 +345,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,7 +409,1762 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>2024-05-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024-05-16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2024-05-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2024-05-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024-05-13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024-05-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024-05-09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2024-05-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2024-05-07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024-05-06</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024-05-03</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024-05-02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024-05-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2024-04-30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024-04-29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2024-04-26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2024-04-25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2024-04-24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2024-04-23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2024-04-22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2024-04-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2024-04-18</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2024-04-17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024-04-16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024-04-15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2024-04-12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2024-04-11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2024-04-10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2024-04-09</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024-04-08</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2024-04-05</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2024-04-04</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2024-04-03</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2024-04-02</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2024-04-01</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2024-03-28</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2024-03-27</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2024-03-26</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2024-03-25</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2024-03-22</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2024-03-21</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2024-03-20</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2024-03-19</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2024-03-18</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2024-03-15</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2024-03-14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2024-03-13</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2024-03-12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2024-03-11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2024-03-08</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2024-03-07</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2024-03-06</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2024-03-05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2024-03-04</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2024-03-01</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2024-02-29</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2024-02-28</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2024-02-27</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2024-02-26</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2024-02-23</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2024-02-22</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2024-02-21</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2024-02-20</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2024-02-16</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2024-02-15</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2024-02-14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>1833859.833333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1826802.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1827880.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1830377.3666666669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1824002.033333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1801534</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1796975.033333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1780485.7666666671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1772159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1746043.1333333331</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1731018.466666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1747563.666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1736590.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1708920.966666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1691543.6333333331</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1744007.466666667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1742337.1333333331</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1706428.6333333331</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1666751.0666666669</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1665577.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1635751.8666666669</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1576537.2666666671</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1456503.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1306266.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1300428.4333333331</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1382711.166666667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1439864.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1457586.3666666669</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1446451.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1451356.533333333</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1436288.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1427884.2333333329</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1404702.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1403083.8666666669</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1392329.666666667</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1390094.1333333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1391075.7666666671</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1402717.166666667</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1406572.7333333329</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1431640.833333333</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1427577.2666666671</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1408636.2666666671</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1395473.7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1411422.166666667</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1434305.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1374409.4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1400729.533333333</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1403065.5666666669</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1386379.966666667</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1368742.6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1376554.033333333</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1369667.6333333331</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1370401.7666666671</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1356758.533333333</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1332115.166666667</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1238397.2333333329</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1171688.5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1160415.466666667</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1162469.8666666669</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1164057.333333333</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1168839.3666666669</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1162192.9333333331</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1185700.033333333</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1181059.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1187171.8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1205652.833333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F8C-4838-A556-4C837F70D003}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="2022020799"/>
+        <c:axId val="2022009983"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>2024-05-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024-05-16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2024-05-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2024-05-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024-05-13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024-05-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024-05-09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2024-05-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2024-05-07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024-05-06</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024-05-03</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024-05-02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024-05-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2024-04-30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024-04-29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2024-04-26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2024-04-25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2024-04-24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2024-04-23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2024-04-22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2024-04-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2024-04-18</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2024-04-17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2024-04-16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024-04-15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2024-04-12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2024-04-11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2024-04-10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2024-04-09</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024-04-08</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2024-04-05</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2024-04-04</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2024-04-03</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2024-04-02</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2024-04-01</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2024-03-28</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2024-03-27</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2024-03-26</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2024-03-25</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2024-03-22</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2024-03-21</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2024-03-20</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2024-03-19</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2024-03-18</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2024-03-15</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2024-03-14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2024-03-13</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2024-03-12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2024-03-11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2024-03-08</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2024-03-07</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2024-03-06</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2024-03-05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2024-03-04</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2024-03-01</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2024-02-29</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2024-02-28</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2024-02-27</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2024-02-26</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2024-02-23</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2024-02-22</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2024-02-21</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2024-02-20</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2024-02-16</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2024-02-15</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2024-02-14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>5.3135885803666259E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3030539310092641E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2996746943394721E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.14114572062234E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5101616419055047E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5112702636353678E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5140667694797453E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3085903167597273E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3186910377930462E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.316717968855935E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2699768420006302E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0954660693794271E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.359287087720721E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.3835628808795777E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3643321377163183E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3982557271127912E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3608584901804597E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.3399858409570573E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.4737095818391382E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.6924612514738938E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.6778980139460131E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.4638216045662887E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.5167675528363408E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.313401070612371E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.3444767915167411E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.3625516449751602E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.3553720403345391E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.3297727156788363E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.9896066565735003E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.9637123406573287E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.9540096146869793E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0563771670927189E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.0752075695843883E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0882160448768483E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6075437044727323E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.6069963792369127E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.7381087807270732E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.8635785741572887E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.9507979846133372E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.0580626204087008E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.0568265827736762E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.0950445924023709E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.9426874694821307E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.9991554887662742E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.0037774293490538E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.9260579691973831E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.9603611837792459E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.887179742595546E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8771690836831208E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.6991342808262289E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.6840021374660902E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.6472746401760433E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.5919709162003733E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.6091049661425671E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.795577584929169E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.6300834695130117E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.6846627501745333E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.6691480721957583E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.6750929336723158E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.6848283922599423E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.7180556513912867E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.6303933410822532E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.756229427922167E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.6614487958538222E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.5669363903489293E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.993752551651393E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9F8C-4838-A556-4C837F70D003}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2043026895"/>
+        <c:axId val="2043036879"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2022020799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2022009983"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2022009983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2022020799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2043036879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2043026895"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2043026895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2043036879"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D46BBA1-DBAF-4B08-8B31-35F5BE1B1E27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,7 +2210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,9 +2242,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,6 +2294,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -670,16 +2487,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -690,10 +2509,19 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>221.21</v>
@@ -702,12 +2530,21 @@
         <v>1541746</v>
       </c>
       <c r="D2">
-        <v>219.2201409953269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>219.22014099532689</v>
+      </c>
+      <c r="E2">
+        <v>1833859.833333333</v>
+      </c>
+      <c r="F2">
+        <v>1479662.666666667</v>
+      </c>
+      <c r="G2">
+        <v>5.3135885803666259E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>220.43</v>
@@ -718,10 +2555,19 @@
       <c r="D3">
         <v>219.7834917927527</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>1826802.1</v>
+      </c>
+      <c r="F3">
+        <v>1472293.0888888889</v>
+      </c>
+      <c r="G3">
+        <v>5.3030539310092641E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>220.24</v>
@@ -730,12 +2576,21 @@
         <v>1251171</v>
       </c>
       <c r="D4">
-        <v>220.423093339891</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>220.42309333989101</v>
+      </c>
+      <c r="E4">
+        <v>1827880.5</v>
+      </c>
+      <c r="F4">
+        <v>1472761.0111111109</v>
+      </c>
+      <c r="G4">
+        <v>5.2996746943394721E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>215.83</v>
@@ -746,10 +2601,19 @@
       <c r="D5">
         <v>221.0541096286866</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1830377.3666666669</v>
+      </c>
+      <c r="F5">
+        <v>1471506.8444444439</v>
+      </c>
+      <c r="G5">
+        <v>5.14114572062234E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>216.65</v>
@@ -758,12 +2622,21 @@
         <v>1465619</v>
       </c>
       <c r="D6">
-        <v>222.0891003171579</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>222.08910031715789</v>
+      </c>
+      <c r="E6">
+        <v>1824002.033333333</v>
+      </c>
+      <c r="F6">
+        <v>1467834.5</v>
+      </c>
+      <c r="G6">
+        <v>5.5101616419055047E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>217.77</v>
@@ -774,10 +2647,19 @@
       <c r="D7">
         <v>222.7836528343808</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1801534</v>
+      </c>
+      <c r="F7">
+        <v>1465760.3222222221</v>
+      </c>
+      <c r="G7">
+        <v>5.5112702636353678E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>218.63</v>
@@ -788,10 +2670,16 @@
       <c r="D8">
         <v>223.5053107198614</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>1796975.033333333</v>
+      </c>
+      <c r="G8">
+        <v>5.5140667694797453E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>213.95</v>
@@ -800,12 +2688,18 @@
         <v>1189663</v>
       </c>
       <c r="D9">
-        <v>224.3370588129573</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>224.33705881295731</v>
+      </c>
+      <c r="E9">
+        <v>1780485.7666666671</v>
+      </c>
+      <c r="G9">
+        <v>5.3085903167597273E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>214.62</v>
@@ -814,12 +2708,18 @@
         <v>1860058</v>
       </c>
       <c r="D10">
-        <v>225.2294700404046</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>225.22947004040461</v>
+      </c>
+      <c r="E10">
+        <v>1772159</v>
+      </c>
+      <c r="G10">
+        <v>5.3186910377930462E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>216.7</v>
@@ -828,12 +2728,18 @@
         <v>1343774</v>
       </c>
       <c r="D11">
-        <v>226.3531114313442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>226.35311143134419</v>
+      </c>
+      <c r="E11">
+        <v>1746043.1333333331</v>
+      </c>
+      <c r="G11">
+        <v>5.316717968855935E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>215.19</v>
@@ -842,12 +2748,18 @@
         <v>1197081</v>
       </c>
       <c r="D12">
-        <v>227.2306967713073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>227.23069677130729</v>
+      </c>
+      <c r="E12">
+        <v>1731018.466666667</v>
+      </c>
+      <c r="G12">
+        <v>5.2699768420006302E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>209.95</v>
@@ -856,12 +2768,18 @@
         <v>1589246</v>
       </c>
       <c r="D13">
-        <v>228.7498346078378</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>228.74983460783781</v>
+      </c>
+      <c r="E13">
+        <v>1747563.666666667</v>
+      </c>
+      <c r="G13">
+        <v>5.0954660693794271E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>210.71</v>
@@ -870,12 +2788,18 @@
         <v>1687750</v>
       </c>
       <c r="D14">
-        <v>230.1379240477245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>230.13792404772451</v>
+      </c>
+      <c r="E14">
+        <v>1736590.5</v>
+      </c>
+      <c r="G14">
+        <v>5.359287087720721E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>212.85</v>
@@ -884,12 +2808,18 @@
         <v>1427716</v>
       </c>
       <c r="D15">
-        <v>231.2133279147745</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>231.21332791477451</v>
+      </c>
+      <c r="E15">
+        <v>1708920.966666667</v>
+      </c>
+      <c r="G15">
+        <v>5.3835628808795777E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>216.78</v>
@@ -898,12 +2828,18 @@
         <v>1437021</v>
       </c>
       <c r="D16">
-        <v>232.1580451510276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>232.15804515102761</v>
+      </c>
+      <c r="E16">
+        <v>1691543.6333333331</v>
+      </c>
+      <c r="G16">
+        <v>5.3643321377163183E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>217.93</v>
@@ -912,12 +2848,18 @@
         <v>1277888</v>
       </c>
       <c r="D17">
-        <v>233.8511939920211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>233.85119399202111</v>
+      </c>
+      <c r="E17">
+        <v>1744007.466666667</v>
+      </c>
+      <c r="G17">
+        <v>5.3982557271127912E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>216.4</v>
@@ -926,12 +2868,18 @@
         <v>2211585</v>
       </c>
       <c r="D18">
-        <v>234.8201147376491</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>234.82011473764911</v>
+      </c>
+      <c r="E18">
+        <v>1742337.1333333331</v>
+      </c>
+      <c r="G18">
+        <v>5.3608584901804597E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>215</v>
@@ -942,10 +2890,16 @@
       <c r="D19">
         <v>236.1450128001251</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>1706428.6333333331</v>
+      </c>
+      <c r="G19">
+        <v>5.3399858409570573E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>217.93</v>
@@ -954,12 +2908,18 @@
         <v>1504576</v>
       </c>
       <c r="D20">
-        <v>238.0223750751262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>238.02237507512621</v>
+      </c>
+      <c r="E20">
+        <v>1666751.0666666669</v>
+      </c>
+      <c r="G20">
+        <v>5.4737095818391382E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>217.13</v>
@@ -970,10 +2930,16 @@
       <c r="D21">
         <v>239.2224956653163</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>1665577.1</v>
+      </c>
+      <c r="G21">
+        <v>5.6924612514738938E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>216.5</v>
@@ -982,12 +2948,18 @@
         <v>3157485</v>
       </c>
       <c r="D22">
-        <v>240.2493326618242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>240.24933266182421</v>
+      </c>
+      <c r="E22">
+        <v>1635751.8666666669</v>
+      </c>
+      <c r="G22">
+        <v>5.6778980139460131E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>210.63</v>
@@ -996,12 +2968,18 @@
         <v>4609060</v>
       </c>
       <c r="D23">
-        <v>242.2316837713826</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>242.23168377138259</v>
+      </c>
+      <c r="E23">
+        <v>1576537.2666666671</v>
+      </c>
+      <c r="G23">
+        <v>5.4638216045662887E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>214.92</v>
@@ -1010,12 +2988,18 @@
         <v>6357444</v>
       </c>
       <c r="D24">
-        <v>245.7696945431512</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>245.76969454315119</v>
+      </c>
+      <c r="E24">
+        <v>1456503.6</v>
+      </c>
+      <c r="G24">
+        <v>5.5167675528363408E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>228.24</v>
@@ -1024,12 +3008,18 @@
         <v>2120161</v>
       </c>
       <c r="D25">
-        <v>250.8462060053303</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>250.84620600533029</v>
+      </c>
+      <c r="E25">
+        <v>1306266.2</v>
+      </c>
+      <c r="G25">
+        <v>5.313401070612371E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>229.62</v>
@@ -1040,10 +3030,16 @@
       <c r="D26">
         <v>252.5660161806162</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>1300428.4333333331</v>
+      </c>
+      <c r="G26">
+        <v>5.3444767915167411E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>236.98</v>
@@ -1054,10 +3050,16 @@
       <c r="D27">
         <v>254.4637183969609</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>1382711.166666667</v>
+      </c>
+      <c r="G27">
+        <v>5.3625516449751602E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>241.06</v>
@@ -1066,12 +3068,18 @@
         <v>1171342</v>
       </c>
       <c r="D28">
-        <v>255.4040901371328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>255.40409013713281</v>
+      </c>
+      <c r="E28">
+        <v>1439864.6</v>
+      </c>
+      <c r="G28">
+        <v>5.3553720403345391E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>239.01</v>
@@ -1080,12 +3088,18 @@
         <v>1285050</v>
       </c>
       <c r="D29">
-        <v>255.7823277696683</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>255.78232776966831</v>
+      </c>
+      <c r="E29">
+        <v>1457586.3666666669</v>
+      </c>
+      <c r="G29">
+        <v>5.3297727156788363E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>247.93</v>
@@ -1094,12 +3108,18 @@
         <v>840676</v>
       </c>
       <c r="D30">
-        <v>256.3046115033046</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>256.30461150330461</v>
+      </c>
+      <c r="E30">
+        <v>1446451.6</v>
+      </c>
+      <c r="G30">
+        <v>4.9896066565735003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>245.89</v>
@@ -1108,12 +3128,18 @@
         <v>1273523</v>
       </c>
       <c r="D31">
-        <v>256.4900241284614</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>256.49002412846141</v>
+      </c>
+      <c r="E31">
+        <v>1451356.533333333</v>
+      </c>
+      <c r="G31">
+        <v>4.9637123406573287E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>244.74</v>
@@ -1122,12 +3148,18 @@
         <v>1330014</v>
       </c>
       <c r="D32">
-        <v>256.8168528580974</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>256.81685285809738</v>
+      </c>
+      <c r="E32">
+        <v>1436288.8</v>
+      </c>
+      <c r="G32">
+        <v>4.9540096146869793E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>244.81</v>
@@ -1136,12 +3168,18 @@
         <v>1437758</v>
       </c>
       <c r="D33">
-        <v>257.1959273785197</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>257.19592737851968</v>
+      </c>
+      <c r="E33">
+        <v>1427884.2333333329</v>
+      </c>
+      <c r="G33">
+        <v>5.0563771670927189E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>246.38</v>
@@ -1150,12 +3188,18 @@
         <v>1326077</v>
       </c>
       <c r="D34">
-        <v>257.536141699755</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>257.53614169975498</v>
+      </c>
+      <c r="E34">
+        <v>1404702.5</v>
+      </c>
+      <c r="G34">
+        <v>5.0752075695843883E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>248.71</v>
@@ -1164,12 +3208,18 @@
         <v>1692080</v>
       </c>
       <c r="D35">
-        <v>257.818521848397</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>257.81852184839698</v>
+      </c>
+      <c r="E35">
+        <v>1403083.8666666669</v>
+      </c>
+      <c r="G35">
+        <v>5.0882160448768483E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>259.44</v>
@@ -1178,12 +3228,18 @@
         <v>791578</v>
       </c>
       <c r="D36">
-        <v>258.2032896758886</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>258.20328967588858</v>
+      </c>
+      <c r="E36">
+        <v>1392329.666666667</v>
+      </c>
+      <c r="G36">
+        <v>4.6075437044727323E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>260.42</v>
@@ -1192,26 +3248,38 @@
         <v>896092</v>
       </c>
       <c r="D37">
-        <v>258.232746326244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>258.23274632624401</v>
+      </c>
+      <c r="E37">
+        <v>1390094.1333333331</v>
+      </c>
+      <c r="G37">
+        <v>4.6069963792369127E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B38">
-        <v>260.97</v>
+        <v>260.97000000000003</v>
       </c>
       <c r="C38">
         <v>992342</v>
       </c>
       <c r="D38">
-        <v>258.2731014054758</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>258.27310140547581</v>
+      </c>
+      <c r="E38">
+        <v>1391075.7666666671</v>
+      </c>
+      <c r="G38">
+        <v>4.7381087807270732E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>261.67</v>
@@ -1222,10 +3290,16 @@
       <c r="D39">
         <v>258.1612661167261</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>1402717.166666667</v>
+      </c>
+      <c r="G39">
+        <v>4.8635785741572887E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>261.57</v>
@@ -1234,12 +3308,18 @@
         <v>1076582</v>
       </c>
       <c r="D40">
-        <v>258.1801391711418</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>258.18013917114178</v>
+      </c>
+      <c r="E40">
+        <v>1406572.7333333329</v>
+      </c>
+      <c r="G40">
+        <v>4.9507979846133372E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B41">
         <v>262.86</v>
@@ -1248,12 +3328,18 @@
         <v>893034</v>
       </c>
       <c r="D41">
-        <v>258.4570613940065</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>258.45706139400647</v>
+      </c>
+      <c r="E41">
+        <v>1431640.833333333</v>
+      </c>
+      <c r="G41">
+        <v>5.0580626204087008E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B42">
         <v>265.75</v>
@@ -1262,12 +3348,18 @@
         <v>1693437</v>
       </c>
       <c r="D42">
-        <v>258.4202211116746</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>258.42022111167461</v>
+      </c>
+      <c r="E42">
+        <v>1427577.2666666671</v>
+      </c>
+      <c r="G42">
+        <v>5.0568265827736762E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B43">
         <v>262.43</v>
@@ -1276,12 +3368,18 @@
         <v>1260051</v>
       </c>
       <c r="D43">
-        <v>258.1267572418979</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>258.12675724189791</v>
+      </c>
+      <c r="E43">
+        <v>1408636.2666666671</v>
+      </c>
+      <c r="G43">
+        <v>5.0950445924023709E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>256.19</v>
@@ -1290,12 +3388,18 @@
         <v>857664</v>
       </c>
       <c r="D44">
-        <v>257.9115382833801</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>257.91153828338008</v>
+      </c>
+      <c r="E44">
+        <v>1395473.7</v>
+      </c>
+      <c r="G44">
+        <v>4.9426874694821307E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <v>255.18</v>
@@ -1304,12 +3408,18 @@
         <v>906396</v>
       </c>
       <c r="D45">
-        <v>257.7854301199511</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>257.78543011995112</v>
+      </c>
+      <c r="E45">
+        <v>1411422.166666667</v>
+      </c>
+      <c r="G45">
+        <v>4.9991554887662742E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>254.24</v>
@@ -1318,26 +3428,38 @@
         <v>3010936</v>
       </c>
       <c r="D46">
-        <v>257.7908766162499</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>257.79087661624988</v>
+      </c>
+      <c r="E46">
+        <v>1434305.3</v>
+      </c>
+      <c r="G46">
+        <v>5.0037774293490538E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B47">
-        <v>258.53</v>
+        <v>258.52999999999997</v>
       </c>
       <c r="C47">
         <v>1227778</v>
       </c>
       <c r="D47">
-        <v>257.9700604288649</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>257.97006042886488</v>
+      </c>
+      <c r="E47">
+        <v>1374409.4</v>
+      </c>
+      <c r="G47">
+        <v>4.9260579691973831E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>258.7</v>
@@ -1346,26 +3468,38 @@
         <v>1134330</v>
       </c>
       <c r="D48">
-        <v>257.7539846317226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>257.75398463172257</v>
+      </c>
+      <c r="E48">
+        <v>1400729.533333333</v>
+      </c>
+      <c r="G48">
+        <v>4.9603611837792459E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>262.78</v>
+        <v>262.77999999999997</v>
       </c>
       <c r="C49">
         <v>1437911</v>
       </c>
       <c r="D49">
-        <v>257.6917509321909</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>257.69175093219093</v>
+      </c>
+      <c r="E49">
+        <v>1403065.5666666669</v>
+      </c>
+      <c r="G49">
+        <v>4.887179742595546E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>258.26</v>
@@ -1374,12 +3508,18 @@
         <v>1469357</v>
       </c>
       <c r="D50">
-        <v>257.5054319216337</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>257.50543192163371</v>
+      </c>
+      <c r="E50">
+        <v>1386379.966666667</v>
+      </c>
+      <c r="G50">
+        <v>4.8771690836831208E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>251.86</v>
@@ -1388,12 +3528,18 @@
         <v>881719</v>
       </c>
       <c r="D51">
-        <v>257.3768690918707</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>257.37686909187067</v>
+      </c>
+      <c r="E51">
+        <v>1368742.6</v>
+      </c>
+      <c r="G51">
+        <v>4.6991342808262289E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>253.84</v>
@@ -1402,12 +3548,18 @@
         <v>1381047</v>
       </c>
       <c r="D52">
-        <v>257.3425901015</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>257.34259010149998</v>
+      </c>
+      <c r="E52">
+        <v>1376554.033333333</v>
+      </c>
+      <c r="G52">
+        <v>4.6840021374660902E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>251.1</v>
@@ -1416,12 +3568,18 @@
         <v>1008050</v>
       </c>
       <c r="D53">
-        <v>257.3264730574904</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>257.32647305749038</v>
+      </c>
+      <c r="E53">
+        <v>1369667.6333333331</v>
+      </c>
+      <c r="G53">
+        <v>4.6472746401760433E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>247.29</v>
@@ -1432,10 +3590,16 @@
       <c r="D54">
         <v>257.3652303649248</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>1370401.7666666671</v>
+      </c>
+      <c r="G54">
+        <v>4.5919709162003733E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>260.7</v>
@@ -1444,12 +3608,18 @@
         <v>1945028</v>
       </c>
       <c r="D55">
-        <v>257.5904571054107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>257.59045710541068</v>
+      </c>
+      <c r="E55">
+        <v>1356758.533333333</v>
+      </c>
+      <c r="G55">
+        <v>3.6091049661425671E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>264.74</v>
@@ -1458,12 +3628,18 @@
         <v>3854244</v>
       </c>
       <c r="D56">
-        <v>257.1690732237741</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>257.16907322377409</v>
+      </c>
+      <c r="E56">
+        <v>1332115.166666667</v>
+      </c>
+      <c r="G56">
+        <v>3.795577584929169E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>258.17</v>
@@ -1472,12 +3648,18 @@
         <v>3331660</v>
       </c>
       <c r="D57">
-        <v>255.9348946028815</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>255.93489460288151</v>
+      </c>
+      <c r="E57">
+        <v>1238397.2333333329</v>
+      </c>
+      <c r="G57">
+        <v>3.6300834695130117E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>255.25</v>
@@ -1486,12 +3668,18 @@
         <v>1702995</v>
       </c>
       <c r="D58">
-        <v>255.0620268825716</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>255.06202688257159</v>
+      </c>
+      <c r="E58">
+        <v>1171688.5</v>
+      </c>
+      <c r="G58">
+        <v>3.6846627501745333E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B59">
         <v>256.95</v>
@@ -1500,26 +3688,38 @@
         <v>951007</v>
       </c>
       <c r="D59">
-        <v>254.5211394057025</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>254.52113940570251</v>
+      </c>
+      <c r="E59">
+        <v>1160415.466666667</v>
+      </c>
+      <c r="G59">
+        <v>3.6691480721957583E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B60">
-        <v>257.35</v>
+        <v>257.35000000000002</v>
       </c>
       <c r="C60">
         <v>987824</v>
       </c>
       <c r="D60">
-        <v>254.1041050443286</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>254.10410504432861</v>
+      </c>
+      <c r="E60">
+        <v>1162469.8666666669</v>
+      </c>
+      <c r="G60">
+        <v>3.6750929336723158E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B61">
         <v>257.2</v>
@@ -1530,10 +3730,16 @@
       <c r="D61">
         <v>253.6133675005126</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>1164057.333333333</v>
+      </c>
+      <c r="G61">
+        <v>3.6848283922599423E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B62">
         <v>256.98</v>
@@ -1542,12 +3748,18 @@
         <v>1077877</v>
       </c>
       <c r="D62">
-        <v>253.1222456701421</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>253.12224567014209</v>
+      </c>
+      <c r="E62">
+        <v>1168839.3666666669</v>
+      </c>
+      <c r="G62">
+        <v>3.7180556513912867E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B63">
         <v>252.52</v>
@@ -1556,12 +3768,18 @@
         <v>742306</v>
       </c>
       <c r="D63">
-        <v>252.5705603650777</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>252.57056036507771</v>
+      </c>
+      <c r="E63">
+        <v>1162192.9333333331</v>
+      </c>
+      <c r="G63">
+        <v>3.6303933410822532E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B64">
         <v>255.26</v>
@@ -1570,12 +3788,18 @@
         <v>1277518</v>
       </c>
       <c r="D64">
-        <v>251.8749149106037</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>251.87491491060371</v>
+      </c>
+      <c r="E64">
+        <v>1185700.033333333</v>
+      </c>
+      <c r="G64">
+        <v>3.756229427922167E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B65">
         <v>258.3</v>
@@ -1586,10 +3810,16 @@
       <c r="D65">
         <v>251.0346800085878</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>1181059.3</v>
+      </c>
+      <c r="G65">
+        <v>3.6614487958538222E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B66">
         <v>261.25</v>
@@ -1598,12 +3828,18 @@
         <v>724512</v>
       </c>
       <c r="D66">
-        <v>249.7911127909204</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>249.79111279092041</v>
+      </c>
+      <c r="E66">
+        <v>1187171.8</v>
+      </c>
+      <c r="G66">
+        <v>3.5669363903489293E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B67">
         <v>262.17</v>
@@ -1614,10 +3850,16 @@
       <c r="D67">
         <v>248.7624132278543</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>1205652.833333333</v>
+      </c>
+      <c r="G67">
+        <v>3.993752551651393E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B68">
         <v>256.76</v>
@@ -1626,20 +3868,20 @@
         <v>1341584</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B69">
-        <v>262.04</v>
+        <v>262.04000000000002</v>
       </c>
       <c r="C69">
         <v>1055527</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B70">
         <v>266.68</v>
@@ -1648,9 +3890,9 @@
         <v>1828625</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B71">
         <v>261.51</v>
@@ -1659,9 +3901,9 @@
         <v>771127</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B72">
         <v>258.43</v>
@@ -1670,9 +3912,9 @@
         <v>1125207</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B73">
         <v>253.98</v>
@@ -1681,9 +3923,9 @@
         <v>865174</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B74">
         <v>252.81</v>
@@ -1692,9 +3934,9 @@
         <v>1336118</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B75">
         <v>256.45</v>
@@ -1703,9 +3945,9 @@
         <v>1592890</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B76">
         <v>255.07</v>
@@ -1714,9 +3956,9 @@
         <v>1214059</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B77">
         <v>253.81</v>
@@ -1725,20 +3967,20 @@
         <v>2017382</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B78">
-        <v>256.47</v>
+        <v>256.47000000000003</v>
       </c>
       <c r="C78">
         <v>1204411</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B79">
         <v>257.23</v>
@@ -1747,9 +3989,9 @@
         <v>937343</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B80">
         <v>253.07</v>
@@ -1758,9 +4000,9 @@
         <v>940236</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B81">
         <v>251.75</v>
@@ -1769,9 +4011,9 @@
         <v>1116062</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B82">
         <v>252.66</v>
@@ -1780,9 +4022,9 @@
         <v>1174455</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B83">
         <v>252.78</v>
@@ -1791,9 +4033,9 @@
         <v>1030074</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B84">
         <v>250.79</v>
@@ -1802,9 +4044,9 @@
         <v>1441025</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B85">
         <v>248.64</v>
@@ -1813,9 +4055,9 @@
         <v>1205727</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B86">
         <v>241.18</v>
@@ -1824,9 +4066,9 @@
         <v>1042706</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B87">
         <v>238.47</v>
@@ -1835,9 +4077,9 @@
         <v>1330398</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B88">
         <v>241.5</v>
@@ -1846,9 +4088,9 @@
         <v>1364804</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B89">
         <v>242.44</v>
@@ -1857,9 +4099,9 @@
         <v>1012639</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B90">
         <v>240.65</v>
@@ -1868,9 +4110,9 @@
         <v>1035448</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B91">
         <v>238.82</v>
@@ -1879,9 +4121,9 @@
         <v>964952</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B92">
         <v>235.96</v>
@@ -1890,9 +4132,9 @@
         <v>878484</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B93">
         <v>235.45</v>
@@ -1901,9 +4143,9 @@
         <v>1447519</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B94">
         <v>229.52</v>
@@ -1912,9 +4154,9 @@
         <v>1138296</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B95">
         <v>228.92</v>
@@ -1923,9 +4165,9 @@
         <v>1552829</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B96">
         <v>227.19</v>
@@ -1934,9 +4176,9 @@
         <v>1278943</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B97">
         <v>234.12</v>
@@ -1947,5 +4189,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>